<commit_message>
Added functions to validator Fixed JSON reading and writing functions Added tests for reading and writing, as well as validating
</commit_message>
<xml_diff>
--- a/tests/test_files/123-ABC.xlsx
+++ b/tests/test_files/123-ABC.xlsx
@@ -1,37 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,10 +69,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -57,14 +88,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -353,62 +385,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>foo</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>bar</t>
-        </is>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B</t>
-        </is>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed instances of dataframes to containers, e.g. 'df' to 'container.df'
</commit_message>
<xml_diff>
--- a/tests/test_files/123-ABC.xlsx
+++ b/tests/test_files/123-ABC.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/workspace/confluence/tests/test_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE48298-1FE6-3348-A41C-5CE2083B8202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
   <si>
     <t>A</t>
   </si>
@@ -30,21 +30,19 @@
   <si>
     <t>C</t>
   </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -60,7 +58,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -68,36 +66,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -144,7 +132,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +164,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +216,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,43 +409,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>